<commit_message>
update mit bahr an salten und umgekehrt
</commit_message>
<xml_diff>
--- a/netzwerke/jung-wien-exp/pivot-tables/jung-wien-alle-without-gaps_pivot.xlsx
+++ b/netzwerke/jung-wien-exp/pivot-tables/jung-wien-alle-without-gaps_pivot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Arthur Schnitzler – Felix Salten</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Hermann Bahr – Hugo von Hofmannsthal</t>
+  </si>
+  <si>
+    <t>Hermann Bahr – Paul Goldmann</t>
   </si>
   <si>
     <t>Hermann Bahr – Richard Beer-Hofmann</t>
@@ -410,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -456,8 +459,11 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>1888</v>
       </c>
@@ -497,8 +503,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1889</v>
       </c>
@@ -538,8 +547,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>1890</v>
       </c>
@@ -574,13 +586,16 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>1891</v>
       </c>
@@ -612,16 +627,19 @@
         <v>28</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>1892</v>
       </c>
@@ -656,13 +674,16 @@
         <v>0</v>
       </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>20</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>1893</v>
       </c>
@@ -697,13 +718,16 @@
         <v>0</v>
       </c>
       <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>22</v>
       </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>1894</v>
       </c>
@@ -735,16 +759,19 @@
         <v>13</v>
       </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>18</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>25</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>1895</v>
       </c>
@@ -776,16 +803,19 @@
         <v>11</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9">
         <v>17</v>
       </c>
-      <c r="M9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>1896</v>
       </c>
@@ -805,7 +835,7 @@
         <v>55</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -817,16 +847,19 @@
         <v>26</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
         <v>8</v>
       </c>
-      <c r="M10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>1897</v>
       </c>
@@ -846,7 +879,7 @@
         <v>51</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -858,16 +891,19 @@
         <v>23</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>1898</v>
       </c>
@@ -887,7 +923,7 @@
         <v>47</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>4</v>
@@ -899,16 +935,19 @@
         <v>37</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
         <v>23</v>
       </c>
-      <c r="M12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>1899</v>
       </c>
@@ -928,7 +967,7 @@
         <v>61</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H13">
         <v>10</v>
@@ -940,16 +979,19 @@
         <v>20</v>
       </c>
       <c r="K13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
         <v>13</v>
       </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>1900</v>
       </c>
@@ -969,7 +1011,7 @@
         <v>38</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -981,16 +1023,19 @@
         <v>30</v>
       </c>
       <c r="K14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
         <v>11</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>1901</v>
       </c>
@@ -1010,7 +1055,7 @@
         <v>41</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H15">
         <v>8</v>
@@ -1025,13 +1070,16 @@
         <v>0</v>
       </c>
       <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>34</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>1902</v>
       </c>
@@ -1063,16 +1111,19 @@
         <v>17</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="M16">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>1903</v>
       </c>
@@ -1092,7 +1143,7 @@
         <v>22</v>
       </c>
       <c r="G17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17">
         <v>14</v>
@@ -1104,16 +1155,19 @@
         <v>29</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>3</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>18</v>
       </c>
-      <c r="M17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>1904</v>
       </c>
@@ -1133,7 +1187,7 @@
         <v>36</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H18">
         <v>14</v>
@@ -1145,16 +1199,19 @@
         <v>28</v>
       </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>13</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>3</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>1905</v>
       </c>
@@ -1174,7 +1231,7 @@
         <v>25</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H19">
         <v>18</v>
@@ -1186,16 +1243,19 @@
         <v>8</v>
       </c>
       <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>13</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>18</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>1906</v>
       </c>
@@ -1215,7 +1275,7 @@
         <v>13</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -1227,16 +1287,19 @@
         <v>10</v>
       </c>
       <c r="K20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>1907</v>
       </c>
@@ -1256,7 +1319,7 @@
         <v>27</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>4</v>
@@ -1268,16 +1331,19 @@
         <v>4</v>
       </c>
       <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
         <v>8</v>
       </c>
-      <c r="L21">
-        <v>4</v>
-      </c>
       <c r="M21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1">
         <v>1908</v>
       </c>
@@ -1297,7 +1363,7 @@
         <v>23</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>4</v>
@@ -1309,16 +1375,19 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1">
         <v>1909</v>
       </c>
@@ -1338,7 +1407,7 @@
         <v>26</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -1350,16 +1419,19 @@
         <v>4</v>
       </c>
       <c r="K23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
         <v>3</v>
       </c>
-      <c r="M23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>1910</v>
       </c>
@@ -1379,7 +1451,7 @@
         <v>33</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1394,13 +1466,16 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1">
         <v>1911</v>
       </c>
@@ -1420,7 +1495,7 @@
         <v>7</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1435,13 +1510,16 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1">
         <v>1912</v>
       </c>
@@ -1461,7 +1539,7 @@
         <v>16</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1473,16 +1551,19 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>2</v>
       </c>
       <c r="M26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1">
         <v>1913</v>
       </c>
@@ -1502,7 +1583,7 @@
         <v>8</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1514,16 +1595,19 @@
         <v>0</v>
       </c>
       <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>6</v>
       </c>
-      <c r="L27">
-        <v>2</v>
-      </c>
       <c r="M27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1">
         <v>1914</v>
       </c>
@@ -1555,16 +1639,19 @@
         <v>16</v>
       </c>
       <c r="K28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
         <v>3</v>
       </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1">
         <v>1915</v>
       </c>
@@ -1599,13 +1686,16 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1">
         <v>1916</v>
       </c>
@@ -1637,16 +1727,19 @@
         <v>20</v>
       </c>
       <c r="K30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1">
         <v>1917</v>
       </c>
@@ -1666,7 +1759,7 @@
         <v>7</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1681,13 +1774,16 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="1">
         <v>1918</v>
       </c>
@@ -1719,16 +1815,19 @@
         <v>17</v>
       </c>
       <c r="K32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
         <v>6</v>
       </c>
-      <c r="M32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="1">
         <v>1919</v>
       </c>
@@ -1760,16 +1859,19 @@
         <v>3</v>
       </c>
       <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
         <v>6</v>
       </c>
-      <c r="L33">
-        <v>4</v>
-      </c>
       <c r="M33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1">
         <v>1920</v>
       </c>
@@ -1801,16 +1903,19 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>4</v>
       </c>
       <c r="M34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1">
         <v>1921</v>
       </c>
@@ -1830,7 +1935,7 @@
         <v>6</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1845,13 +1950,16 @@
         <v>0</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="1">
         <v>1922</v>
       </c>
@@ -1886,13 +1994,16 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1">
         <v>1923</v>
       </c>
@@ -1924,16 +2035,19 @@
         <v>5</v>
       </c>
       <c r="K37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="1">
         <v>1924</v>
       </c>
@@ -1968,13 +2082,16 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>4</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1">
         <v>1925</v>
       </c>
@@ -1994,7 +2111,7 @@
         <v>6</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H39">
         <v>11</v>
@@ -2006,16 +2123,19 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <v>2</v>
       </c>
       <c r="M39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="1">
         <v>1926</v>
       </c>
@@ -2050,13 +2170,16 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1">
         <v>1927</v>
       </c>
@@ -2076,7 +2199,7 @@
         <v>3</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H41">
         <v>4</v>
@@ -2091,13 +2214,16 @@
         <v>0</v>
       </c>
       <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
         <v>5</v>
       </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1">
         <v>1928</v>
       </c>
@@ -2137,8 +2263,11 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1">
         <v>1929</v>
       </c>
@@ -2173,13 +2302,16 @@
         <v>0</v>
       </c>
       <c r="L43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>2</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="1">
         <v>1930</v>
       </c>
@@ -2219,8 +2351,11 @@
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="1">
         <v>1931</v>
       </c>
@@ -2258,6 +2393,9 @@
         <v>0</v>
       </c>
       <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
         <v>0</v>
       </c>
     </row>

</xml_diff>